<commit_message>
a few recheck BIS labels
</commit_message>
<xml_diff>
--- a/01_Data/counts_MASTER.xlsx
+++ b/01_Data/counts_MASTER.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8961" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8976" uniqueCount="1113">
   <si>
     <t>site</t>
   </si>
@@ -3365,6 +3365,9 @@
   </si>
   <si>
     <t>Recheck</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -66809,7 +66812,7 @@
         <v>1B-02M-EA</v>
       </c>
       <c r="G66" s="16" t="b">
-        <f t="shared" ref="G66:G97" si="5">IF(E66="","",F66=A66)</f>
+        <f t="shared" ref="G66:G82" si="5">IF(E66="","",F66=A66)</f>
         <v>1</v>
       </c>
       <c r="H66" s="16">
@@ -67835,9 +67838,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P259"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67904,7 +67907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>248</v>
       </c>
@@ -67947,7 +67950,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -67990,7 +67993,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>250</v>
       </c>
@@ -68077,7 +68080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>251</v>
       </c>
@@ -68860,7 +68863,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -68870,7 +68873,9 @@
       <c r="C25" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E25" s="19"/>
       <c r="F25">
         <v>-76.414015000000006</v>
@@ -68906,7 +68911,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>323</v>
       </c>
@@ -68916,7 +68921,9 @@
       <c r="C26" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E26" s="19"/>
       <c r="F26">
         <v>-76.414015000000006</v>
@@ -69034,7 +69041,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -69044,7 +69051,9 @@
       <c r="C29" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E29" s="19"/>
       <c r="F29">
         <v>-76.420936999999995</v>
@@ -69080,7 +69089,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>258</v>
       </c>
@@ -69090,7 +69099,9 @@
       <c r="C30" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E30" s="19"/>
       <c r="F30">
         <v>-76.420936999999995</v>
@@ -69123,7 +69134,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -69133,7 +69144,9 @@
       <c r="C31" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E31" s="19"/>
       <c r="F31">
         <v>-76.414799000000002</v>
@@ -69169,7 +69182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>259</v>
       </c>
@@ -69179,7 +69192,9 @@
       <c r="C32" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E32" s="19"/>
       <c r="F32">
         <v>-76.414799000000002</v>
@@ -69212,7 +69227,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -69222,7 +69237,9 @@
       <c r="C33" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E33" s="19"/>
       <c r="F33">
         <v>-76.420468999999997</v>
@@ -69258,7 +69275,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>260</v>
       </c>
@@ -69268,7 +69285,9 @@
       <c r="C34" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>834</v>
+      </c>
       <c r="E34" s="19"/>
       <c r="F34">
         <v>-76.420468999999997</v>
@@ -69301,7 +69320,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -69311,7 +69330,9 @@
       <c r="C35" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E35" s="19"/>
       <c r="F35">
         <v>-76.415925999999999</v>
@@ -69347,7 +69368,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>261</v>
       </c>
@@ -69357,7 +69378,9 @@
       <c r="C36" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E36" s="19"/>
       <c r="F36">
         <v>-76.415925999999999</v>
@@ -69390,7 +69413,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>100</v>
       </c>
@@ -69400,7 +69423,9 @@
       <c r="C37" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E37" s="19"/>
       <c r="F37">
         <v>-76.418719999999993</v>
@@ -69436,7 +69461,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>262</v>
       </c>
@@ -69446,7 +69471,9 @@
       <c r="C38" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E38" s="19"/>
       <c r="F38">
         <v>-76.418719999999993</v>
@@ -69807,7 +69834,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -69817,7 +69844,9 @@
       <c r="C47" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D47" s="19"/>
+      <c r="D47" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E47" s="19"/>
       <c r="F47">
         <v>-76.411698999999999</v>
@@ -69853,7 +69882,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -69863,7 +69892,9 @@
       <c r="C48" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E48" s="19"/>
       <c r="F48">
         <v>-76.411755999999997</v>
@@ -69896,7 +69927,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -69906,7 +69937,9 @@
       <c r="C49" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="D49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>1112</v>
+      </c>
       <c r="E49" s="14"/>
       <c r="F49">
         <v>-76.411653999999999</v>
@@ -69939,7 +69972,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -70026,7 +70059,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -70072,7 +70105,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>264</v>
       </c>
@@ -70115,7 +70148,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -70161,7 +70194,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -70207,7 +70240,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -70297,7 +70330,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -70343,7 +70376,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>108</v>
       </c>
@@ -70389,7 +70422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>265</v>
       </c>
@@ -70435,7 +70468,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -70481,7 +70514,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>266</v>
       </c>
@@ -70522,7 +70555,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>111</v>
       </c>
@@ -70568,7 +70601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>113</v>
       </c>
@@ -70655,7 +70688,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>268</v>
       </c>
@@ -70824,7 +70857,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>116</v>
       </c>
@@ -70870,7 +70903,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>270</v>
       </c>
@@ -70913,7 +70946,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>117</v>
       </c>
@@ -71243,7 +71276,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>120</v>
       </c>
@@ -71330,7 +71363,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>121</v>
       </c>
@@ -71631,7 +71664,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>275</v>
       </c>
@@ -71759,7 +71792,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>125</v>
       </c>
@@ -71805,7 +71838,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>277</v>
       </c>
@@ -71892,7 +71925,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>128</v>
       </c>
@@ -71938,7 +71971,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>130</v>
       </c>
@@ -71984,7 +72017,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -72027,7 +72060,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>131</v>
       </c>
@@ -72073,7 +72106,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>132</v>
       </c>
@@ -72251,7 +72284,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>136</v>
       </c>
@@ -72297,7 +72330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>137</v>
       </c>
@@ -72343,7 +72376,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>138</v>
       </c>
@@ -72389,7 +72422,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>139</v>
       </c>
@@ -72435,7 +72468,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>140</v>
       </c>
@@ -72481,7 +72514,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>44</v>
       </c>
@@ -72527,7 +72560,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>154</v>
       </c>
@@ -72573,7 +72606,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>279</v>
       </c>
@@ -72616,7 +72649,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>155</v>
       </c>
@@ -72832,7 +72865,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>282</v>
       </c>
@@ -72960,7 +72993,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>245</v>
       </c>
@@ -73047,7 +73080,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>159</v>
       </c>
@@ -73178,7 +73211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>286</v>
       </c>
@@ -73265,7 +73298,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>287</v>
       </c>
@@ -73308,7 +73341,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>162</v>
       </c>
@@ -73354,7 +73387,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>288</v>
       </c>
@@ -73644,7 +73677,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>53</v>
       </c>
@@ -73856,7 +73889,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>175</v>
       </c>
@@ -73943,7 +73976,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>176</v>
       </c>
@@ -73989,7 +74022,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>291</v>
       </c>
@@ -74032,7 +74065,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>177</v>
       </c>
@@ -74122,7 +74155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>292</v>
       </c>
@@ -74467,7 +74500,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>296</v>
       </c>
@@ -74598,7 +74631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>185</v>
       </c>
@@ -74644,7 +74677,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>194</v>
       </c>
@@ -74690,7 +74723,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>297</v>
       </c>
@@ -74733,7 +74766,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>298</v>
       </c>
@@ -74776,7 +74809,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="161" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>195</v>
       </c>
@@ -74822,7 +74855,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>299</v>
       </c>
@@ -74865,7 +74898,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>196</v>
       </c>
@@ -74911,7 +74944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>197</v>
       </c>
@@ -74957,7 +74990,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>198</v>
       </c>
@@ -75003,7 +75036,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>199</v>
       </c>
@@ -75049,7 +75082,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="167" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>200</v>
       </c>
@@ -75095,7 +75128,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>201</v>
       </c>
@@ -75141,7 +75174,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>202</v>
       </c>
@@ -75187,7 +75220,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>203</v>
       </c>
@@ -75233,7 +75266,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>300</v>
       </c>
@@ -75276,7 +75309,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>204</v>
       </c>
@@ -75322,7 +75355,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>205</v>
       </c>
@@ -75368,7 +75401,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="174" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>206</v>
       </c>
@@ -75414,7 +75447,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>207</v>
       </c>
@@ -75460,7 +75493,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>208</v>
       </c>
@@ -75506,7 +75539,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>301</v>
       </c>
@@ -75549,7 +75582,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>209</v>
       </c>
@@ -75595,7 +75628,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>210</v>
       </c>
@@ -75641,7 +75674,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>211</v>
       </c>
@@ -75687,7 +75720,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>212</v>
       </c>
@@ -75733,7 +75766,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>213</v>
       </c>
@@ -75779,7 +75812,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>214</v>
       </c>
@@ -75825,7 +75858,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>215</v>
       </c>
@@ -75871,7 +75904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>216</v>
       </c>
@@ -75917,7 +75950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>302</v>
       </c>
@@ -76130,7 +76163,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>219</v>
       </c>
@@ -76217,7 +76250,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>220</v>
       </c>
@@ -76433,7 +76466,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>308</v>
       </c>
@@ -76764,7 +76797,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>228</v>
       </c>
@@ -76810,7 +76843,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>312</v>
       </c>
@@ -76853,7 +76886,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>313</v>
       </c>
@@ -76896,7 +76929,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>314</v>
       </c>
@@ -76937,7 +76970,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>229</v>
       </c>
@@ -76983,7 +77016,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>315</v>
       </c>
@@ -77572,7 +77605,7 @@
   <autoFilter ref="A1:P220">
     <filterColumn colId="2">
       <filters>
-        <filter val="0"/>
+        <filter val="x"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>